<commit_message>
Fixed Crowdstrike excel file assumption
</commit_message>
<xml_diff>
--- a/public/models/crowdstrike.xlsx
+++ b/public/models/crowdstrike.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bp/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE7E8D-63B4-AA4E-A4BC-1D8A745FE25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66755D2-A66D-A243-A8C9-54B4001E5EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{E3D15AAA-CE64-634F-96BA-2AF8CAD2DB42}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E3D15AAA-CE64-634F-96BA-2AF8CAD2DB42}"/>
   </bookViews>
   <sheets>
     <sheet name="CrowdStrike Financials" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
   <si>
     <t>CrowdStrike Holdings, Inc.</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t>29.0x</t>
+  </si>
+  <si>
+    <t>28x</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B50987-9614-A448-A39A-ABB44E220FE8}">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3879,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4285CFDA-0315-4C21-9E0E-2E0A7A3CEB1B}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3954,7 +3957,7 @@
         <v>87</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
         <v>81</v>
@@ -3970,7 +3973,7 @@
       </c>
       <c r="F7" s="61">
         <f>VALUE(LEFT(F6,LEN(F6)-1))*F5</f>
-        <v>17498.292375316953</v>
+        <v>25786.957184677616</v>
       </c>
       <c r="H7" t="s">
         <v>90</v>
@@ -4044,7 +4047,7 @@
       </c>
       <c r="F12" s="58">
         <f>F7</f>
-        <v>17498.292375316953</v>
+        <v>25786.957184677616</v>
       </c>
       <c r="H12" t="s">
         <v>81</v>
@@ -4060,7 +4063,7 @@
       </c>
       <c r="F14" s="56">
         <f>((F12*F11)-F10*(1+F11)^0.5)/(F12+F10*(1+F11)^0.5)</f>
-        <v>-2.6382925051504757E-3</v>
+        <v>3.0109484787151291E-2</v>
       </c>
       <c r="H14" s="52" t="s">
         <v>92</v>
@@ -4245,7 +4248,7 @@
       </c>
       <c r="I27" s="76" t="str">
         <f>F6</f>
-        <v>19.0x</v>
+        <v>28x</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4261,7 +4264,7 @@
       <c r="H28" s="68"/>
       <c r="I28" s="69">
         <f>VALUE(LEFT(I27,LEN(I27)-1))*I26</f>
-        <v>17498.292375316953</v>
+        <v>25786.957184677616</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4286,7 +4289,7 @@
       <c r="H30" s="68"/>
       <c r="I30" s="78">
         <f>I28*I29</f>
-        <v>10533.858223891732</v>
+        <v>15523.580540472027</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4320,7 +4323,7 @@
       </c>
       <c r="M33" s="9">
         <f>F43</f>
-        <v>15286.531143609009</v>
+        <v>20276.253460189306</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4369,7 +4372,7 @@
       </c>
       <c r="F37" s="76" t="str">
         <f>F6</f>
-        <v>19.0x</v>
+        <v>28x</v>
       </c>
       <c r="H37" t="s">
         <v>105</v>
@@ -4384,7 +4387,7 @@
       </c>
       <c r="F38" s="61">
         <f>VALUE(LEFT(F37,LEN(F37)-1))*F36</f>
-        <v>17498.292375316953</v>
+        <v>25786.957184677616</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -4400,7 +4403,7 @@
       </c>
       <c r="M39" s="81">
         <f>M33-M34-M36+M37</f>
-        <v>17835.492143609008</v>
+        <v>22825.214460189305</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -4409,7 +4412,7 @@
       </c>
       <c r="F40" s="60">
         <f>F38*F39</f>
-        <v>10533.858223891732</v>
+        <v>15523.580540472027</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -4418,7 +4421,7 @@
       </c>
       <c r="F41" s="7">
         <f>I30/F43</f>
-        <v>0.68909408713668341</v>
+        <v>0.76560398946241492</v>
       </c>
       <c r="H41" s="107" t="s">
         <v>109</v>
@@ -4435,7 +4438,7 @@
       </c>
       <c r="M42" s="9">
         <f>F43</f>
-        <v>15286.531143609009</v>
+        <v>20276.253460189306</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -4444,7 +4447,7 @@
       </c>
       <c r="F43" s="81">
         <f>F33+F40</f>
-        <v>15286.531143609009</v>
+        <v>20276.253460189306</v>
       </c>
       <c r="H43" t="s">
         <v>110</v>
@@ -4460,7 +4463,7 @@
       </c>
       <c r="M45" s="83">
         <f>M42/M43</f>
-        <v>73.546256898903195</v>
+        <v>97.552710416830962</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>